<commit_message>
adding product to the cart scenario optimized
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/ModaMerve.xlsx
+++ b/src/test/java/apachePOI/ModaMerve.xlsx
@@ -3,25 +3,28 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nebahatozcan/Desktop/JavaDemos/Selenium_Automation_Framework/src/test/java/apachePOI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A7F8B9-0345-3247-BEF1-6AC96EFF8318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF03FA40-1A01-5245-9CE7-482A223F5331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Information" sheetId="1" r:id="rId1"/>
-    <sheet name="20230708_235954" r:id="rId5" sheetId="2"/>
+    <sheet name="20230708_235954" sheetId="2" r:id="rId2"/>
+    <sheet name="20230711_135242" sheetId="3" r:id="rId3"/>
+    <sheet name="20230711_135722" sheetId="4" r:id="rId4"/>
+    <sheet name="20230711_145932" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="41">
   <si>
     <t>Product Link</t>
   </si>
@@ -150,7 +153,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -498,167 +500,170 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.5"/>
-    <col min="2" max="2" customWidth="true" width="24.5"/>
-    <col min="3" max="3" customWidth="true" width="29.0"/>
-    <col min="5" max="5" customWidth="true" width="33.6640625"/>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -668,168 +673,675 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s" s="0">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s" s="0">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s" s="0">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s" s="0">
+      <c r="D9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s" s="0">
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s" s="0">
+      <c r="D10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s" s="0">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="D11" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>